<commit_message>
Column width fixed; Labs are now functional
</commit_message>
<xml_diff>
--- a/globals.xlsx
+++ b/globals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\r studio\r_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\TreatMeta\r_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E7315FE-83A2-4F58-BA76-178D9824CC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454271DC-90CD-422D-8E09-39429B113CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{D5FC97F5-EF2E-4254-A4B2-5AC9B147C8F4}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="3" xr2:uid="{D5FC97F5-EF2E-4254-A4B2-5AC9B147C8F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="91">
   <si>
     <t>Function</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t>text</t>
+  </si>
+  <si>
+    <t>autocomplete</t>
   </si>
 </sst>
 </file>
@@ -2445,8 +2448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003599B1-E80F-4279-81E3-4F2640C97B1E}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2998,7 +3001,7 @@
         <v>81</v>
       </c>
       <c r="H35" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Lab Category; Modified Context Menu
</commit_message>
<xml_diff>
--- a/globals.xlsx
+++ b/globals.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\TreatMeta\r_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C2D343-BBF2-4AF7-83A3-441CBF60D603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C519702-E05F-4835-B1AC-7AB1061E6425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{D5FC97F5-EF2E-4254-A4B2-5AC9B147C8F4}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="109">
   <si>
     <t>Function</t>
   </si>
@@ -301,9 +301,6 @@
     <t>EsP</t>
   </si>
   <si>
-    <t>EsC</t>
-  </si>
-  <si>
     <t>EsD</t>
   </si>
   <si>
@@ -344,6 +341,33 @@
   </si>
   <si>
     <t>SD change</t>
+  </si>
+  <si>
+    <t>Lab Conversions</t>
+  </si>
+  <si>
+    <t>calculate_sm</t>
+  </si>
+  <si>
+    <t>SE of TE</t>
+  </si>
+  <si>
+    <t>apply_labs</t>
+  </si>
+  <si>
+    <t>lab_apply</t>
+  </si>
+  <si>
+    <t>lab_output</t>
+  </si>
+  <si>
+    <t>Converted Values</t>
+  </si>
+  <si>
+    <t>Labs</t>
+  </si>
+  <si>
+    <t>Values to be converted</t>
   </si>
 </sst>
 </file>
@@ -733,10 +757,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A9188BC-DF61-45E0-9330-C784012EB633}">
-  <dimension ref="A1:X15"/>
+  <dimension ref="A1:Y17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +768,7 @@
     <col min="1" max="1" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -817,8 +841,11 @@
       <c r="X1" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="Y1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -853,7 +880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -882,7 +909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -917,7 +944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -952,7 +979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -975,7 +1002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1004,7 +1031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1027,7 +1054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1047,7 +1074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1097,7 +1124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1117,86 +1144,117 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="K12">
-        <v>1</v>
-      </c>
-      <c r="X12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="X13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="X13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>65</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="X14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="X15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>66</v>
       </c>
-      <c r="W15">
-        <v>1</v>
-      </c>
-      <c r="X15">
+      <c r="W16">
+        <v>1</v>
+      </c>
+      <c r="X16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="X17">
+        <v>1</v>
+      </c>
+      <c r="Y17">
         <v>1</v>
       </c>
     </row>
@@ -1207,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FFC011-93B8-40BC-A6EB-1563586BDB38}">
-  <dimension ref="A1:AC26"/>
+  <dimension ref="A1:AD28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD1" sqref="AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,7 +1277,7 @@
     <col min="9" max="9" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1307,8 +1365,11 @@
       <c r="AC1" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD1" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1337,7 +1398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1372,7 +1433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1407,7 +1468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1433,7 +1494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1465,7 +1526,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1497,7 +1558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1529,7 +1590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1567,7 +1628,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1605,7 +1666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -1637,7 +1698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -1675,7 +1736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -1713,7 +1774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -1751,7 +1812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -1789,7 +1850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1824,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1850,7 +1911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -1876,7 +1937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>11</v>
       </c>
@@ -1908,7 +1969,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1943,15 +2004,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -1960,7 +2021,7 @@
         <v>0</v>
       </c>
       <c r="F21">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21">
         <v>1</v>
@@ -1975,7 +2036,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -1983,10 +2044,10 @@
         <v>0</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -2007,61 +2068,70 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>66</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>4</v>
       </c>
-      <c r="AB23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="AB24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>9</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -2075,11 +2145,8 @@
       <c r="G25">
         <v>1</v>
       </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2087,10 +2154,10 @@
         <v>0</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>1</v>
@@ -2104,13 +2171,65 @@
       <c r="H26">
         <v>1</v>
       </c>
-      <c r="I26">
-        <v>1</v>
-      </c>
-      <c r="J26">
-        <v>1</v>
-      </c>
-      <c r="K26">
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>103</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="AC28">
+        <v>1</v>
+      </c>
+      <c r="AD28">
         <v>1</v>
       </c>
     </row>
@@ -2121,10 +2240,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63FE69D-38BB-4D46-B519-F8C9B6D3DD48}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I17" sqref="B17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,7 +2252,7 @@
     <col min="8" max="8" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2153,7 +2272,7 @@
         <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>34</v>
@@ -2161,8 +2280,11 @@
       <c r="I1" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2190,8 +2312,11 @@
       <c r="I2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2219,8 +2344,11 @@
       <c r="I3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -2248,8 +2376,11 @@
       <c r="I4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -2277,8 +2408,11 @@
       <c r="I5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -2306,8 +2440,11 @@
       <c r="I6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -2335,8 +2472,11 @@
       <c r="I7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -2364,8 +2504,11 @@
       <c r="I8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -2393,8 +2536,11 @@
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -2422,8 +2568,11 @@
       <c r="I10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -2451,120 +2600,199 @@
       <c r="I11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>65</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>66</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
         <v>1</v>
       </c>
     </row>
@@ -2575,21 +2803,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003599B1-E80F-4279-81E3-4F2640C97B1E}">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="I53" sqref="I53:I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="17.42578125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1"/>
-    <col min="7" max="7" width="40" customWidth="1"/>
-    <col min="8" max="27" width="18" customWidth="1"/>
+    <col min="6" max="6" width="17.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="31.140625" customWidth="1"/>
+    <col min="8" max="8" width="40" customWidth="1"/>
+    <col min="9" max="28" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>27</v>
       </c>
@@ -2602,609 +2830,998 @@
       <c r="D1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E2" s="3" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>41</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" t="s">
+        <v>60</v>
+      </c>
+      <c r="I11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="I12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+      <c r="I16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" t="s">
+        <v>44</v>
+      </c>
+      <c r="I19" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" t="s">
+        <v>44</v>
+      </c>
+      <c r="I24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>3</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G27" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" t="s">
+        <v>44</v>
+      </c>
+      <c r="I28" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F30" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G30" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G31" t="s">
+        <v>62</v>
+      </c>
+      <c r="I31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" t="s">
+        <v>47</v>
+      </c>
+      <c r="I32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F33" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G33" t="s">
+        <v>48</v>
+      </c>
+      <c r="I33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G35" t="s">
+        <v>49</v>
+      </c>
+      <c r="I35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F36" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G37" t="s">
+        <v>51</v>
+      </c>
+      <c r="I37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F38" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+      <c r="I38" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F39" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G39" t="s">
+        <v>53</v>
+      </c>
+      <c r="I39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F40" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G40" t="s">
+        <v>54</v>
+      </c>
+      <c r="I40" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F41" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G41" t="s">
+        <v>55</v>
+      </c>
+      <c r="I41" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="42" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" t="s">
+        <v>56</v>
+      </c>
+      <c r="I42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="43" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G43" t="s">
+        <v>57</v>
+      </c>
+      <c r="I43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F44" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G44" t="s">
+        <v>91</v>
+      </c>
+      <c r="I44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F45" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="G45" t="s">
+        <v>92</v>
+      </c>
+      <c r="I45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F46" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G46" t="s">
+        <v>98</v>
+      </c>
+      <c r="I46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F47" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G47" t="s">
+        <v>96</v>
+      </c>
+      <c r="I47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F48" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G48" t="s">
+        <v>97</v>
+      </c>
+      <c r="I48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F49" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G49" t="s">
+        <v>99</v>
+      </c>
+      <c r="I49" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="50" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F50" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G50" t="s">
+        <v>64</v>
+      </c>
+      <c r="I50" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" t="s">
+        <v>72</v>
+      </c>
+      <c r="I51" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="52" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F52" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" t="s">
+        <v>31</v>
+      </c>
+      <c r="I52" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="53" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F53" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G53" t="s">
+        <v>102</v>
+      </c>
+      <c r="I53" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F54" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G54" t="s">
+        <v>108</v>
+      </c>
+      <c r="I54" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="55" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F55" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G55" t="s">
+        <v>106</v>
+      </c>
+      <c r="I55" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="56" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F56" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G56" t="s">
+        <v>80</v>
+      </c>
+      <c r="I56" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E3" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E4" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F11" t="s">
-        <v>60</v>
-      </c>
-      <c r="H11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
-        <v>60</v>
-      </c>
-      <c r="H13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" t="s">
-        <v>44</v>
-      </c>
-      <c r="H14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
-        <v>44</v>
-      </c>
-      <c r="H16" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" t="s">
-        <v>45</v>
-      </c>
-      <c r="H17" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E18" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F18" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E19" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" t="s">
-        <v>62</v>
-      </c>
-      <c r="H19" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" t="s">
-        <v>47</v>
-      </c>
-      <c r="H20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" t="s">
-        <v>48</v>
-      </c>
-      <c r="H21" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E22" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" t="s">
-        <v>49</v>
-      </c>
-      <c r="H23" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E24" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F25" t="s">
-        <v>51</v>
-      </c>
-      <c r="H25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E26" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" t="s">
-        <v>52</v>
-      </c>
-      <c r="H26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E27" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F27" t="s">
-        <v>53</v>
-      </c>
-      <c r="H27" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E28" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F28" t="s">
-        <v>54</v>
-      </c>
-      <c r="H28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="29" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E29" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" t="s">
-        <v>55</v>
-      </c>
-      <c r="H29" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E30" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" t="s">
-        <v>56</v>
-      </c>
-      <c r="H30" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E31" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F31" t="s">
-        <v>57</v>
-      </c>
-      <c r="H31" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="32" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E32" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F32" t="s">
-        <v>92</v>
-      </c>
-      <c r="H32" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F33" t="s">
-        <v>93</v>
-      </c>
-      <c r="H33" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E34" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F34" t="s">
-        <v>99</v>
-      </c>
-      <c r="H34" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E35" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F35" t="s">
-        <v>97</v>
-      </c>
-      <c r="H35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E36" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F36" t="s">
-        <v>98</v>
-      </c>
-      <c r="H36" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="37" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E37" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F37" t="s">
-        <v>100</v>
-      </c>
-      <c r="H37" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E38" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F38" t="s">
-        <v>64</v>
-      </c>
-      <c r="H38" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="39" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E39" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F39" t="s">
-        <v>72</v>
-      </c>
-      <c r="H39" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E40" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F40" t="s">
-        <v>80</v>
-      </c>
-      <c r="H40" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E41" s="3"/>
-    </row>
-    <row r="42" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E42" s="3"/>
-    </row>
-    <row r="43" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E43" s="3"/>
-    </row>
-    <row r="44" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E44" s="3"/>
-    </row>
-    <row r="45" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E45" s="3"/>
-    </row>
-    <row r="46" spans="5:8" x14ac:dyDescent="0.25">
-      <c r="E46" s="3"/>
+    <row r="59" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F60" s="3"/>
+    </row>
+    <row r="61" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F61" s="3"/>
+    </row>
+    <row r="62" spans="6:9" x14ac:dyDescent="0.25">
+      <c r="F62" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3213,10 +3830,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11D1C26F-6FDD-42BA-A71C-9885E5C52A64}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3264,6 +3881,14 @@
         <v>78</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3273,11 +3898,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC55B6A7-04F0-43D0-9771-5F1DA7C24A5A}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView zoomScale="142" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -3290,10 +3918,10 @@
         <v>85</v>
       </c>
       <c r="D1" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" t="s">
         <v>86</v>
-      </c>
-      <c r="E1" t="s">
-        <v>87</v>
       </c>
       <c r="F1" t="s">
         <v>83</v>
@@ -3313,7 +3941,7 @@
         <v>2</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -3336,7 +3964,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -3382,7 +4010,7 @@
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -3401,18 +4029,16 @@
       <c r="C6" t="s">
         <v>61</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>30</v>
+      <c r="D6" t="s">
+        <v>79</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3421,77 +4047,68 @@
       <c r="C7" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
       <c r="E7" t="s">
         <v>61</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
-      <c r="D8" t="s">
-        <v>15</v>
+      <c r="C8" t="s">
+        <v>14</v>
       </c>
       <c r="E8" t="s">
         <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="D9" t="s">
-        <v>61</v>
-      </c>
-      <c r="F9" t="s">
-        <v>61</v>
+      <c r="C9" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" t="s">
-        <v>79</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
output has become wide; Rename variables needs a more generic algorithm
</commit_message>
<xml_diff>
--- a/globals.xlsx
+++ b/globals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\TreatMeta\r_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C519702-E05F-4835-B1AC-7AB1061E6425}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6298219F-8FF1-49E1-9270-522880253479}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{D5FC97F5-EF2E-4254-A4B2-5AC9B147C8F4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D5FC97F5-EF2E-4254-A4B2-5AC9B147C8F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="109">
   <si>
     <t>Function</t>
   </si>
@@ -1267,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66FFC011-93B8-40BC-A6EB-1563586BDB38}">
   <dimension ref="A1:AD28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AD1" sqref="AD1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1420,9 +1420,6 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
       <c r="M3">
         <v>1</v>
       </c>
@@ -1453,9 +1450,6 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
         <v>1</v>
       </c>
       <c r="M4">
@@ -1516,9 +1510,6 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
       <c r="L6">
         <v>1</v>
       </c>
@@ -1548,9 +1539,6 @@
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
       <c r="L7">
         <v>1</v>
       </c>
@@ -1612,9 +1600,6 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
       <c r="M9">
         <v>1</v>
       </c>
@@ -1650,9 +1635,6 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
       <c r="M10">
         <v>1</v>
       </c>
@@ -1720,9 +1702,6 @@
       <c r="G12">
         <v>1</v>
       </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
       <c r="M12">
         <v>1</v>
       </c>
@@ -1758,9 +1737,6 @@
       <c r="G13">
         <v>1</v>
       </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
       <c r="M13">
         <v>1</v>
       </c>
@@ -1796,9 +1772,6 @@
       <c r="G14">
         <v>1</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
       <c r="J14">
         <v>1</v>
       </c>
@@ -1834,9 +1807,6 @@
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
       <c r="N15">
         <v>1</v>
       </c>
@@ -1870,9 +1840,6 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
         <v>1</v>
       </c>
       <c r="L16">
@@ -2805,8 +2772,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{003599B1-E80F-4279-81E3-4F2640C97B1E}">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53:I54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3896,10 +3863,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC55B6A7-04F0-43D0-9771-5F1DA7C24A5A}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView zoomScale="142" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3955,7 +3922,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -4024,7 +3991,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>61</v>
@@ -4042,7 +4009,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>35</v>
@@ -4056,7 +4023,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -4070,7 +4037,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -4078,36 +4045,41 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>